<commit_message>
adicionando alterações de media
</commit_message>
<xml_diff>
--- a/gerador_bob_esponja/trezentosteste999.xlsx
+++ b/gerador_bob_esponja/trezentosteste999.xlsx
@@ -327,12 +327,12 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
+      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -341,17 +341,16 @@
       </c>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="n">
-        <f aca="false">_xlfn.ORG.LIBREOFFICE.RANDBETWEEN.NV(0,14)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="n">
         <v>2</v>
       </c>
@@ -361,187 +360,169 @@
       </c>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="n">
-        <f aca="false">_xlfn.ORG.LIBREOFFICE.RANDBETWEEN.NV(0,14)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="n">
-        <f aca="false">_xlfn.ORG.LIBREOFFICE.RANDBETWEEN.NV(0,14)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="n">
-        <f aca="false">_xlfn.ORG.LIBREOFFICE.RANDBETWEEN.NV(0,14)</f>
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="n">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="n">
-        <f aca="false">_xlfn.ORG.LIBREOFFICE.RANDBETWEEN.NV(0,14)</f>
         <v>0</v>
       </c>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="n">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="n">
-        <f aca="false">_xlfn.ORG.LIBREOFFICE.RANDBETWEEN.NV(0,14)</f>
         <v>0</v>
       </c>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="n">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="n">
-        <f aca="false">_xlfn.ORG.LIBREOFFICE.RANDBETWEEN.NV(0,14)</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="n">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="n">
-        <f aca="false">_xlfn.ORG.LIBREOFFICE.RANDBETWEEN.NV(0,14)</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="n">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="n">
-        <f aca="false">_xlfn.ORG.LIBREOFFICE.RANDBETWEEN.NV(0,14)</f>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="n">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="n">
-        <f aca="false">_xlfn.ORG.LIBREOFFICE.RANDBETWEEN.NV(0,14)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="n">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="n">
-        <f aca="false">_xlfn.ORG.LIBREOFFICE.RANDBETWEEN.NV(0,14)</f>
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="n">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="n">
-        <f aca="false">_xlfn.ORG.LIBREOFFICE.RANDBETWEEN.NV(0,14)</f>
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="n">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="n">
-        <f aca="false">_xlfn.ORG.LIBREOFFICE.RANDBETWEEN.NV(0,14)</f>
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="n">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="n">
-        <f aca="false">_xlfn.ORG.LIBREOFFICE.RANDBETWEEN.NV(0,14)</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D16" s="2"/>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="n">
         <v>16</v>
       </c>
       <c r="B17" s="2" t="n">
-        <f aca="false">_xlfn.ORG.LIBREOFFICE.RANDBETWEEN.NV(0,14)</f>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="n">
         <v>17</v>
       </c>
       <c r="B18" s="2" t="n">
-        <f aca="false">_xlfn.ORG.LIBREOFFICE.RANDBETWEEN.NV(0,14)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="n">
         <v>18</v>
       </c>
       <c r="B19" s="2" t="n">
-        <f aca="false">_xlfn.ORG.LIBREOFFICE.RANDBETWEEN.NV(0,14)</f>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="n">
         <v>19</v>
       </c>
       <c r="B20" s="2" t="n">
-        <f aca="false">_xlfn.ORG.LIBREOFFICE.RANDBETWEEN.NV(0,14)</f>
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="n">
         <v>20</v>
       </c>
       <c r="B21" s="2" t="n">
-        <f aca="false">_xlfn.ORG.LIBREOFFICE.RANDBETWEEN.NV(0,14)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="n">
         <v>21</v>
       </c>

</xml_diff>